<commit_message>
evidence.xlsx + Stage-1 Tasks A1-A6
</commit_message>
<xml_diff>
--- a/OlegBirkoff/evidence.xlsx
+++ b/OlegBirkoff/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10755"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>TxHash</t>
   </si>
@@ -78,18 +78,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -138,25 +126,52 @@
     <t>uptick1rzrj0646uz58nnnxjr7a3exmucgpmeqq3ly5ce</t>
   </si>
   <si>
-    <t>98EB190FA5D5D937750F293022F5B08E29559053764F0C69C95918A8C5FD411F</t>
-  </si>
-  <si>
-    <t>olegBirkoffGoN</t>
-  </si>
-  <si>
-    <t>olegBirkoff2GoN</t>
-  </si>
-  <si>
-    <t>83F797CEEB0F6FB23D7A3B95F71F04984DCF93541C38296AD95DD27C50A2FBA9</t>
-  </si>
-  <si>
-    <t>968B4CD9BD7F9EAE08E91226306F36D294FD2824B6C596423BF01701B7D49E7C</t>
-  </si>
-  <si>
-    <t>olegBirkoffGoN2</t>
-  </si>
-  <si>
-    <t>D823C94845FA3CCD448F7C6AE158E6BC3428CFA6C34B99CEB0BECFCEA09A0B65</t>
+    <t>C372AD12E2C95D0CF271A37A2B6F73D27737FBAC124F37C50373489F94D93D56</t>
+  </si>
+  <si>
+    <t>birkoffGoNnft</t>
+  </si>
+  <si>
+    <t>7A344EDB75ECFCE187A71FCC8F9B4DB43F0C149D654D3D6821CC41DE80CBBEC1</t>
+  </si>
+  <si>
+    <t>birkoff001</t>
+  </si>
+  <si>
+    <t>47814F4B1B4BD28230997BEED0F7FB1FA668D94C12F2BBEFC015512C9AC703F7</t>
+  </si>
+  <si>
+    <t>birkoff002</t>
+  </si>
+  <si>
+    <t>464D91C4A2FAA94244C29D60F94E5E106288CA0161DC8605B698ED8A63C250EB</t>
+  </si>
+  <si>
+    <t>birkoff003</t>
+  </si>
+  <si>
+    <t>68E5FEB2B0BD4630131E7C0808E9D7A45EC09F3563D7D1A3DF9A8626DC55EB36</t>
+  </si>
+  <si>
+    <t>wasm.juno19us6395gfz2ehej6yj4hzv52zzpmwt55xy6e6xapd2a8lp3twltqpprnz7</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>0AB1D6CEE20724E8A552371CA2F4576F232C12D16E4AEDEBA83331126A8CC4F8</t>
+  </si>
+  <si>
+    <t>ibc/145C27B96C1C9E3111F1B3602A56D8BD52BC6808E5A5F5BF60627C1D1D9E72B5</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>E6567D765DADE5C28C3253F82051E896CB13658797305BCB3F5C24679E74B85D</t>
+  </si>
+  <si>
+    <t>B3DAD9026D48303ACA9F519D9F9EEF5AA927D6CDAC63E00983709E9245442428</t>
   </si>
 </sst>
 </file>
@@ -561,8 +576,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,54 +594,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1071,10 +1086,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,22 +1107,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1348,10 +1356,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,24 +1381,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>36</v>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1405,7 +1424,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1430,16 +1451,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1454,7 +1475,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1479,16 +1502,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1503,7 +1526,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1526,18 +1551,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1577,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1576,18 +1603,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stage-1 A7-A20 tasks - edited
</commit_message>
<xml_diff>
--- a/OlegBirkoff/evidence.xlsx
+++ b/OlegBirkoff/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10755" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10755" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,15 +57,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
@@ -295,6 +286,30 @@
   </si>
   <si>
     <t>E4EFCD0DE0003449A1545DF6CA1798EE490D60E875604296DC24ABB943C10588</t>
+  </si>
+  <si>
+    <t>D2D9CC2D807EB42E456A058624A21E2A2D2B585E57A5EBEECB4553131B8A2029</t>
+  </si>
+  <si>
+    <t>E9E9220FEE3CCE1F349D9FD4189D0E910459D7A19D6D3F4E0F926D642567DA03</t>
+  </si>
+  <si>
+    <t>1F00BC6307035293B00F53C9D4744B720A4BABE8395465C5A906E2CA0D45FC96</t>
+  </si>
+  <si>
+    <t>944A672AA6010D615FAA52B683EF7784A127979806E64DD289D7AD769626BB6F</t>
+  </si>
+  <si>
+    <t>E830781205E55C90C59DD36C1A3DD957D35EF0E6DF60C23C625C9315C1A2C006</t>
+  </si>
+  <si>
+    <t>6FB1B6905B98189D5F914DCCDF382F25E93BA76D28E88C0952C7E45AB62721FA</t>
+  </si>
+  <si>
+    <t>2296E7533A42D753E43134C6BD483F89A4594441086741A784F6EF9723704F14</t>
+  </si>
+  <si>
+    <t>F2190559C9E5B83D7BA56A430DC7786408F56CE4C3CBFB54144AFE8BD6BFCF44</t>
   </si>
 </sst>
 </file>
@@ -717,54 +732,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -791,18 +806,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -829,18 +844,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -855,7 +870,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -867,18 +882,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -905,18 +920,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -951,34 +966,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1013,34 +1028,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1053,9 +1068,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1073,26 +1090,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1101,9 +1131,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1121,23 +1153,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1171,23 +1215,85 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>35</v>
@@ -1195,23 +1301,61 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1233,80 +1377,58 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1333,128 +1455,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1620,43 +1664,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1687,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1698,16 +1742,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1738,10 +1782,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1749,16 +1793,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1789,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1800,16 +1844,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1841,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1852,16 +1896,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1888,18 +1932,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1927,18 +1971,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>